<commit_message>
Made distance scores less scale-dependent
</commit_message>
<xml_diff>
--- a/doc/Class2.xlsx
+++ b/doc/Class2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\cygwin64\home\s.hein\GitHub\Trains\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B6284F32-3D66-4D87-BA19-E7D4CB32E8F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D509DF3D-1064-4176-93A6-5C21C39444C0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="0" windowWidth="27315" windowHeight="12008" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4455" yWindow="0" windowWidth="27315" windowHeight="12008" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="count" sheetId="1" r:id="rId1"/>
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:AP41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection sqref="A1:AP41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1286,10 +1286,10 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="12">
-        <v>14648</v>
+        <v>14653</v>
       </c>
       <c r="E3" s="12">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1315,10 +1315,10 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="E4" s="6">
-        <v>14671</v>
+        <v>14668</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1346,13 +1346,13 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
-        <v>15692</v>
+        <v>15694</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -1376,12 +1376,12 @@
       <c r="E6" s="6"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12">
-        <v>15692</v>
+        <v>15698</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -1460,11 +1460,13 @@
       <c r="F9" s="12">
         <v>4</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6">
+        <v>2</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="12">
-        <v>15696</v>
+        <v>15694</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -1492,16 +1494,16 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="12">
-        <v>9999</v>
+        <v>10301</v>
       </c>
       <c r="L10" s="6">
-        <v>4903</v>
+        <v>5222</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="12">
-        <v>798</v>
+        <v>177</v>
       </c>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
@@ -1523,16 +1525,16 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="12">
-        <v>5045</v>
+        <v>5125</v>
       </c>
       <c r="L11" s="6">
-        <v>9826</v>
+        <v>10381</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="12">
-        <v>829</v>
+        <v>194</v>
       </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
@@ -1556,10 +1558,10 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6">
-        <v>11205</v>
+        <v>11197</v>
       </c>
       <c r="N12" s="6">
-        <v>4195</v>
+        <v>4203</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
@@ -1585,10 +1587,10 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6">
-        <v>4260</v>
+        <v>4314</v>
       </c>
       <c r="N13" s="6">
-        <v>11140</v>
+        <v>11086</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
@@ -1639,16 +1641,16 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="L15" s="6">
-        <v>50</v>
+        <v>220</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6">
-        <v>15611</v>
+        <v>15292</v>
       </c>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
@@ -1676,10 +1678,10 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="12">
-        <v>15319</v>
+        <v>15343</v>
       </c>
       <c r="R16" s="12">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="S16" s="7"/>
     </row>
@@ -1705,10 +1707,10 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="12">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="R17" s="12">
-        <v>15341</v>
+        <v>15329</v>
       </c>
       <c r="S17" s="7"/>
     </row>
@@ -1764,11 +1766,9 @@
       </c>
       <c r="T20" s="5"/>
       <c r="U20" s="12">
-        <v>15799</v>
-      </c>
-      <c r="V20" s="12">
-        <v>1</v>
-      </c>
+        <v>15800</v>
+      </c>
+      <c r="V20" s="12"/>
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="7"/>
@@ -1782,10 +1782,10 @@
       </c>
       <c r="T21" s="5"/>
       <c r="U21" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V21" s="12">
-        <v>15799</v>
+        <v>15797</v>
       </c>
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
@@ -1886,10 +1886,10 @@
         <v>15800</v>
       </c>
       <c r="AC28" s="2">
-        <v>15780</v>
+        <v>15782</v>
       </c>
       <c r="AD28" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AE28" s="3"/>
       <c r="AF28" s="3"/>
@@ -1912,10 +1912,10 @@
         <v>15800</v>
       </c>
       <c r="AC29" s="11">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="AD29" s="6">
-        <v>15784</v>
+        <v>15777</v>
       </c>
       <c r="AE29" s="6"/>
       <c r="AF29" s="6"/>
@@ -2232,7 +2232,7 @@
   <dimension ref="A1:AP41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2547,11 +2547,11 @@
       </c>
       <c r="D3" s="15">
         <f>IF(count!D3 = 0, "", count!D3/$B3)</f>
-        <v>0.95116883116883122</v>
+        <v>0.9514935064935065</v>
       </c>
       <c r="E3" s="17">
         <f>IF(count!E3 = 0, "", count!E3/$B3)</f>
-        <v>4.8831168831168829E-2</v>
+        <v>4.8506493506493505E-2</v>
       </c>
       <c r="F3" s="13" t="str">
         <f>IF(count!F3 = 0, "", count!F3/$B3)</f>
@@ -2715,11 +2715,11 @@
       </c>
       <c r="D4" s="20">
         <f>IF(count!D4 = 0, "", count!D4/$B4)</f>
-        <v>4.7337662337662338E-2</v>
+        <v>4.753246753246753E-2</v>
       </c>
       <c r="E4" s="22">
         <f>IF(count!E4 = 0, "", count!E4/$B4)</f>
-        <v>0.95266233766233765</v>
+        <v>0.95246753246753246</v>
       </c>
       <c r="F4" s="13" t="str">
         <f>IF(count!F4 = 0, "", count!F4/$B4)</f>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="F5" s="15">
         <f>IF(count!F5 = 0, "", count!F5/$B5)</f>
-        <v>0.99949044585987257</v>
+        <v>0.99961783439490448</v>
       </c>
       <c r="G5" s="17" t="str">
         <f>IF(count!G5 = 0, "", count!G5/$B5)</f>
@@ -2905,9 +2905,9 @@
         <f>IF(count!I5 = 0, "", count!I5/$B5)</f>
         <v/>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="23">
         <f>IF(count!J5 = 0, "", count!J5/$B5)</f>
-        <v>5.0955414012738849E-4</v>
+        <v>3.8216560509554139E-4</v>
       </c>
       <c r="K5" s="13" t="str">
         <f>IF(count!K5 = 0, "", count!K5/$B5)</f>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="G6" s="22">
         <f>IF(count!G6 = 0, "", count!G6/$B6)</f>
-        <v>0.99949044585987257</v>
+        <v>0.9998726114649682</v>
       </c>
       <c r="H6" s="13" t="str">
         <f>IF(count!H6 = 0, "", count!H6/$B6)</f>
@@ -3073,9 +3073,9 @@
         <f>IF(count!I6 = 0, "", count!I6/$B6)</f>
         <v/>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="23">
         <f>IF(count!J6 = 0, "", count!J6/$B6)</f>
-        <v>5.0955414012738849E-4</v>
+        <v>1.2738853503184712E-4</v>
       </c>
       <c r="K6" s="13" t="str">
         <f>IF(count!K6 = 0, "", count!K6/$B6)</f>
@@ -3561,13 +3561,13 @@
         <f>IF(count!E9 = 0, "", count!E9/$B9)</f>
         <v/>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="23">
         <f>IF(count!F9 = 0, "", count!F9/$B9)</f>
         <v>2.5477707006369424E-4</v>
       </c>
-      <c r="G9" s="13" t="str">
+      <c r="G9" s="23">
         <f>IF(count!G9 = 0, "", count!G9/$B9)</f>
-        <v/>
+        <v>1.2738853503184712E-4</v>
       </c>
       <c r="H9" s="13" t="str">
         <f>IF(count!H9 = 0, "", count!H9/$B9)</f>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="J9" s="14">
         <f>IF(count!J9 = 0, "", count!J9/$B9)</f>
-        <v>0.99974522292993628</v>
+        <v>0.99961783439490448</v>
       </c>
       <c r="K9" s="13" t="str">
         <f>IF(count!K9 = 0, "", count!K9/$B9)</f>
@@ -3751,11 +3751,11 @@
       </c>
       <c r="K10" s="15">
         <f>IF(count!K10 = 0, "", count!K10/$B10)</f>
-        <v>0.63687898089171979</v>
+        <v>0.65611464968152866</v>
       </c>
       <c r="L10" s="17">
         <f>IF(count!L10 = 0, "", count!L10/$B10)</f>
-        <v>0.31229299363057322</v>
+        <v>0.33261146496815286</v>
       </c>
       <c r="M10" s="13" t="str">
         <f>IF(count!M10 = 0, "", count!M10/$B10)</f>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="P10" s="23">
         <f>IF(count!P10 = 0, "", count!P10/$B10)</f>
-        <v>5.0828025477707005E-2</v>
+        <v>1.1273885350318471E-2</v>
       </c>
       <c r="Q10" s="13" t="str">
         <f>IF(count!Q10 = 0, "", count!Q10/$B10)</f>
@@ -3919,11 +3919,11 @@
       </c>
       <c r="K11" s="20">
         <f>IF(count!K11 = 0, "", count!K11/$B11)</f>
-        <v>0.32133757961783438</v>
+        <v>0.32643312101910826</v>
       </c>
       <c r="L11" s="22">
         <f>IF(count!L11 = 0, "", count!L11/$B11)</f>
-        <v>0.62585987261146492</v>
+        <v>0.66121019108280255</v>
       </c>
       <c r="M11" s="13" t="str">
         <f>IF(count!M11 = 0, "", count!M11/$B11)</f>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="P11" s="23">
         <f>IF(count!P11 = 0, "", count!P11/$B11)</f>
-        <v>5.2802547770700634E-2</v>
+        <v>1.2356687898089172E-2</v>
       </c>
       <c r="Q11" s="13" t="str">
         <f>IF(count!Q11 = 0, "", count!Q11/$B11)</f>
@@ -4095,11 +4095,11 @@
       </c>
       <c r="M12" s="15">
         <f>IF(count!M12 = 0, "", count!M12/$B12)</f>
-        <v>0.72759740259740258</v>
+        <v>0.7270779220779221</v>
       </c>
       <c r="N12" s="17">
         <f>IF(count!N12 = 0, "", count!N12/$B12)</f>
-        <v>0.27240259740259742</v>
+        <v>0.2729220779220779</v>
       </c>
       <c r="O12" s="13" t="str">
         <f>IF(count!O12 = 0, "", count!O12/$B12)</f>
@@ -4263,11 +4263,11 @@
       </c>
       <c r="M13" s="20">
         <f>IF(count!M13 = 0, "", count!M13/$B13)</f>
-        <v>0.2766233766233766</v>
+        <v>0.28012987012987012</v>
       </c>
       <c r="N13" s="22">
         <f>IF(count!N13 = 0, "", count!N13/$B13)</f>
-        <v>0.72337662337662334</v>
+        <v>0.71987012987012988</v>
       </c>
       <c r="O13" s="13" t="str">
         <f>IF(count!O13 = 0, "", count!O13/$B13)</f>
@@ -4589,13 +4589,13 @@
         <f>IF(count!J15 = 0, "", count!J15/$B15)</f>
         <v/>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="23">
         <f>IF(count!K15 = 0, "", count!K15/$B15)</f>
-        <v>2.4840764331210191E-3</v>
-      </c>
-      <c r="L15" s="13">
+        <v>1.1974522292993631E-2</v>
+      </c>
+      <c r="L15" s="23">
         <f>IF(count!L15 = 0, "", count!L15/$B15)</f>
-        <v>3.1847133757961785E-3</v>
+        <v>1.4012738853503185E-2</v>
       </c>
       <c r="M15" s="13" t="str">
         <f>IF(count!M15 = 0, "", count!M15/$B15)</f>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="P15" s="14">
         <f>IF(count!P15 = 0, "", count!P15/$B15)</f>
-        <v>0.99433121019108284</v>
+        <v>0.97401273885350315</v>
       </c>
       <c r="Q15" s="13" t="str">
         <f>IF(count!Q15 = 0, "", count!Q15/$B15)</f>
@@ -4783,11 +4783,11 @@
       </c>
       <c r="Q16" s="15">
         <f>IF(count!Q16 = 0, "", count!Q16/$B16)</f>
-        <v>0.9947402597402597</v>
+        <v>0.99629870129870135</v>
       </c>
       <c r="R16" s="17">
         <f>IF(count!R16 = 0, "", count!R16/$B16)</f>
-        <v>5.2597402597402594E-3</v>
+        <v>3.7012987012987014E-3</v>
       </c>
       <c r="S16" s="19" t="str">
         <f>IF(count!S16 = 0, "", count!S16/$B16)</f>
@@ -4951,11 +4951,11 @@
       </c>
       <c r="Q17" s="20">
         <f>IF(count!Q17 = 0, "", count!Q17/$B17)</f>
-        <v>3.8311688311688311E-3</v>
+        <v>4.6103896103896107E-3</v>
       </c>
       <c r="R17" s="22">
         <f>IF(count!R17 = 0, "", count!R17/$B17)</f>
-        <v>0.99616883116883115</v>
+        <v>0.99538961038961038</v>
       </c>
       <c r="S17" s="19" t="str">
         <f>IF(count!S17 = 0, "", count!S17/$B17)</f>
@@ -5471,11 +5471,11 @@
       </c>
       <c r="U20" s="15">
         <f>IF(count!U20 = 0, "", count!U20/$B20)</f>
-        <v>0.99993670886075947</v>
-      </c>
-      <c r="V20" s="17">
+        <v>1</v>
+      </c>
+      <c r="V20" s="17" t="str">
         <f>IF(count!V20 = 0, "", count!V20/$B20)</f>
-        <v>6.3291139240506333E-5</v>
+        <v/>
       </c>
       <c r="W20" s="13" t="str">
         <f>IF(count!W20 = 0, "", count!W20/$B20)</f>
@@ -5639,11 +5639,11 @@
       </c>
       <c r="U21" s="20">
         <f>IF(count!U21 = 0, "", count!U21/$B21)</f>
-        <v>6.3291139240506333E-5</v>
+        <v>1.8987341772151899E-4</v>
       </c>
       <c r="V21" s="22">
         <f>IF(count!V21 = 0, "", count!V21/$B21)</f>
-        <v>0.99993670886075947</v>
+        <v>0.99981012658227852</v>
       </c>
       <c r="W21" s="13" t="str">
         <f>IF(count!W21 = 0, "", count!W21/$B21)</f>
@@ -6847,11 +6847,11 @@
       </c>
       <c r="AC28" s="15">
         <f>IF(count!AC28 = 0, "", count!AC28/$B28)</f>
-        <v>0.99873417721518987</v>
+        <v>0.99886075949367092</v>
       </c>
       <c r="AD28" s="17">
         <f>IF(count!AD28 = 0, "", count!AD28/$B28)</f>
-        <v>1.2658227848101266E-3</v>
+        <v>1.139240506329114E-3</v>
       </c>
       <c r="AE28" s="16" t="str">
         <f>IF(count!AE28 = 0, "", count!AE28/$B28)</f>
@@ -7015,11 +7015,11 @@
       </c>
       <c r="AC29" s="20">
         <f>IF(count!AC29 = 0, "", count!AC29/$B29)</f>
-        <v>1.0126582278481013E-3</v>
+        <v>1.4556962025316456E-3</v>
       </c>
       <c r="AD29" s="22">
         <f>IF(count!AD29 = 0, "", count!AD29/$B29)</f>
-        <v>0.99898734177215187</v>
+        <v>0.99854430379746839</v>
       </c>
       <c r="AE29" s="13" t="str">
         <f>IF(count!AE29 = 0, "", count!AE29/$B29)</f>

</xml_diff>